<commit_message>
Edited order list for components
</commit_message>
<xml_diff>
--- a/PCB/PCAP04_Interface/bom/Farnell_Order_List.xlsx
+++ b/PCB/PCAP04_Interface/bom/Farnell_Order_List.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Universiteit\Master\Thesis\Measurements\PCAP04\PCB\PCAP04_Interface\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsalden\Thesis\Measurements\PCAP04\PCB\PCAP04_Interface\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05978BBB-BECB-4D0B-8C92-637748594F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EverythingMouser" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
   <si>
     <t>Part Number</t>
   </si>
@@ -154,17 +154,153 @@
   </si>
   <si>
     <t>18650 battery holder</t>
+  </si>
+  <si>
+    <t>Manufactuer number</t>
+  </si>
+  <si>
+    <t>77-VJ0603A1R0BXACBC</t>
+  </si>
+  <si>
+    <t>VJ0603A1R0BXACW1BC</t>
+  </si>
+  <si>
+    <t>VJ0603D2R0BXPAJ</t>
+  </si>
+  <si>
+    <t>77-VJ0603D2R0BXPAJ</t>
+  </si>
+  <si>
+    <t>791-0603B103K101CT</t>
+  </si>
+  <si>
+    <t>0603B103K101CT</t>
+  </si>
+  <si>
+    <t>81-R188R60J106KE7D</t>
+  </si>
+  <si>
+    <t>GRM188R60J106KE47D</t>
+  </si>
+  <si>
+    <t>810-C1608X7S1A475MAC</t>
+  </si>
+  <si>
+    <t>C1608X7S1A475M080AC</t>
+  </si>
+  <si>
+    <t>80-C0603C104J4R</t>
+  </si>
+  <si>
+    <t>C0603C104J4RACTU</t>
+  </si>
+  <si>
+    <t>667-ERA-3AEB64R9V</t>
+  </si>
+  <si>
+    <t>ERA-3AEB64R9V</t>
+  </si>
+  <si>
+    <t>710-150080RS75000</t>
+  </si>
+  <si>
+    <t>150080RS75000</t>
+  </si>
+  <si>
+    <t>710-970250321</t>
+  </si>
+  <si>
+    <t>48SM003</t>
+  </si>
+  <si>
+    <t>M3 screw</t>
+  </si>
+  <si>
+    <t>506-FSM2JSMAATR</t>
+  </si>
+  <si>
+    <t>FSM2JSMAATR</t>
+  </si>
+  <si>
+    <t>579-MCP9701-E/TO</t>
+  </si>
+  <si>
+    <t>MCP9701-E/TO</t>
+  </si>
+  <si>
+    <t>PCAP04-AQFM-24</t>
+  </si>
+  <si>
+    <t>2MS1T2B3M2QES</t>
+  </si>
+  <si>
+    <t>538-43045-2022</t>
+  </si>
+  <si>
+    <t>MEM2067-02-180-00-A</t>
+  </si>
+  <si>
+    <t>485-4684</t>
+  </si>
+  <si>
+    <t>2020 RGB LEDs - 10-pack - WS2812B</t>
+  </si>
+  <si>
+    <t>637-LDI1117-3.3H</t>
+  </si>
+  <si>
+    <t>LDI1117-3.3H</t>
+  </si>
+  <si>
+    <t>3.3 LDO</t>
+  </si>
+  <si>
+    <t>538-43025-2000</t>
+  </si>
+  <si>
+    <t>43025-2000</t>
+  </si>
+  <si>
+    <t>Mouser recepticle</t>
+  </si>
+  <si>
+    <t>538-43030-0004-CT</t>
+  </si>
+  <si>
+    <t>43030-0004 (Cut Strip)</t>
+  </si>
+  <si>
+    <t>Mouser contacts</t>
+  </si>
+  <si>
+    <t>F981A226MMALZT</t>
+  </si>
+  <si>
+    <t>581-F981A226MMALZT</t>
+  </si>
+  <si>
+    <t>Surface mount talantum Cap 22uF</t>
+  </si>
+  <si>
+    <t>Mouser number</t>
+  </si>
+  <si>
+    <t>Shopping cart link</t>
+  </si>
+  <si>
+    <t>https://nl.mouser.com/ProjectManager/ProjectDetail.aspx?AccessID=6550a5fe31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="_ &quot;€&quot;\ * #,##0.0000_ ;_ &quot;€&quot;\ * \-#,##0.0000_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ &quot;€&quot;\ * #,##0.0000_ ;_ &quot;€&quot;\ * \-#,##0.0000_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ &quot;€&quot;\ * #,##0.000_ ;_ &quot;€&quot;\ * \-#,##0.000_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -199,9 +335,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -232,18 +373,29 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -252,7 +404,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{828E8D3D-E85F-4F37-9EE3-7722A9C32C3D}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -341,23 +493,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -393,23 +528,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,14 +703,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
@@ -608,7 +726,7 @@
     <col min="14" max="14" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -643,7 +761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>2896375</v>
       </c>
@@ -673,14 +791,14 @@
         <v>8.35</v>
       </c>
       <c r="N2" s="5">
-        <f>K2*M2</f>
+        <f t="shared" ref="N2:N7" si="1">K2*M2</f>
         <v>8.35</v>
       </c>
       <c r="Q2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2134025</v>
       </c>
@@ -710,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="N3" s="5">
-        <f>K3*M3</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q3" s="8">
@@ -718,7 +836,7 @@
         <v>145.488</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>2672793</v>
       </c>
@@ -748,11 +866,11 @@
         <v>0.5</v>
       </c>
       <c r="N4" s="5">
-        <f>K4*M4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>2494230</v>
       </c>
@@ -782,11 +900,11 @@
         <v>4</v>
       </c>
       <c r="N5" s="5">
-        <f>K5*M5</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6" s="3">
         <v>3416132</v>
       </c>
@@ -800,7 +918,7 @@
         <v>0.113</v>
       </c>
       <c r="E6" s="7">
-        <f t="shared" ref="E6:E15" si="1">D6*B6</f>
+        <f t="shared" ref="E6:E15" si="2">D6*B6</f>
         <v>1.1300000000000001</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -816,11 +934,11 @@
         <v>1.5</v>
       </c>
       <c r="N6" s="5">
-        <f>K6*M6</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>2672791</v>
       </c>
@@ -834,7 +952,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.47199999999999998</v>
       </c>
       <c r="J7" t="s">
@@ -850,11 +968,11 @@
         <v>2.5</v>
       </c>
       <c r="N7" s="5">
-        <f>K7*M7</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>197427</v>
       </c>
@@ -868,11 +986,11 @@
         <v>0.3</v>
       </c>
       <c r="E8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>2331324</v>
       </c>
@@ -886,11 +1004,11 @@
         <v>0.39900000000000002</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="A10" s="3">
         <v>3796325</v>
       </c>
@@ -904,11 +1022,11 @@
         <v>0.121</v>
       </c>
       <c r="E10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>1466783</v>
       </c>
@@ -922,11 +1040,11 @@
         <v>0.46100000000000002</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.6880000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>3397776</v>
       </c>
@@ -940,11 +1058,11 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.8499999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>1439483</v>
       </c>
@@ -958,28 +1076,28 @@
         <v>0.48</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17">
       <c r="E14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17">
       <c r="E15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -996,7 +1114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1014,7 +1132,7 @@
         <v>68.600000000000009</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1032,9 +1150,9 @@
         <v>6.34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>35</v>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1050,7 +1168,7 @@
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1068,12 +1186,12 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1208,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1110,11 +1228,546 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{5374FE2C-649A-40E4-8D06-A40C801005AD}"/>
-    <hyperlink ref="J4" r:id="rId2" xr:uid="{B8A78455-C9B2-41DE-A1FB-BFD0895516EC}"/>
-    <hyperlink ref="J5" r:id="rId3" xr:uid="{23088F65-7E63-4931-A82E-6041523895FA}"/>
-    <hyperlink ref="J6" r:id="rId4" xr:uid="{0B56800D-CC6C-40DF-B6CC-A2E880C22DBF}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J4" r:id="rId2"/>
+    <hyperlink ref="J5" r:id="rId3"/>
+    <hyperlink ref="J6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <f>Sheet1!B2</f>
+        <v>30</v>
+      </c>
+      <c r="D2" t="str">
+        <f>Sheet1!C2</f>
+        <v>SMD Multilayer Ceramic Capacitor, 1 pF</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.114</v>
+      </c>
+      <c r="F2" s="5">
+        <f t="shared" ref="F2:F11" si="0">E2*C2</f>
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <f>Sheet1!B3</f>
+        <v>6</v>
+      </c>
+      <c r="D3" t="str">
+        <f>Sheet1!C3</f>
+        <v>SMD Multilayer Ceramic Capacitor, 2 pF</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.47</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" si="0"/>
+        <v>2.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="str">
+        <f>Sheet1!C4</f>
+        <v>SMD Multilayer Ceramic Capacitor, IR Reflow, 10000</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <f>Sheet1!B5</f>
+        <v>10</v>
+      </c>
+      <c r="D5" t="str">
+        <f>Sheet1!C5</f>
+        <v>SMD Multilayer Ceramic Capacitor, 10 µF</v>
+      </c>
+      <c r="E5" s="11">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <f>Sheet1!B6</f>
+        <v>10</v>
+      </c>
+      <c r="D6" t="str">
+        <f>Sheet1!C6</f>
+        <v>SMD Multilayer Ceramic Capacitor, 4.7 µF</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="0"/>
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <f>Sheet1!B7</f>
+        <v>2</v>
+      </c>
+      <c r="D7" t="str">
+        <f>Sheet1!C7</f>
+        <v>SMD Multilayer Ceramic Capacitor, IR Reflow, 0.1 µF</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <f>Sheet1!B9</f>
+        <v>2</v>
+      </c>
+      <c r="D9" t="str">
+        <f>Sheet1!C9</f>
+        <v>SMD Chip Resistor, 64.9 ohm</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.35</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10">
+        <f>Sheet1!B10</f>
+        <v>5</v>
+      </c>
+      <c r="D10" t="str">
+        <f>Sheet1!C10</f>
+        <v>LED, Red, SMD</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="3">
+        <v>970250321</v>
+      </c>
+      <c r="C11">
+        <f>Sheet1!B11</f>
+        <v>8</v>
+      </c>
+      <c r="D11" t="str">
+        <f>Sheet1!C11</f>
+        <v>Standoff, Zinc Plated</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="str">
+        <f>Sheet1!C12</f>
+        <v>Tactile Switch, FSMJSM</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.32</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ref="F12:F14" si="1">E12*C12</f>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <f>Sheet1!B13</f>
+        <v>2</v>
+      </c>
+      <c r="D13" t="str">
+        <f>Sheet1!C13</f>
+        <v>Temperature Sensor IC, Voltage, ± 2°C, 0 °C, 70 °C, TO-92, 3 Pins</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="1"/>
+        <v>1.552</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="str">
+        <f>Sheet1!A21</f>
+        <v>985-PCAP04-AQFM-24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15">
+        <f>Sheet1!B21</f>
+        <v>10</v>
+      </c>
+      <c r="D15" t="str">
+        <f>Sheet1!C21</f>
+        <v>PCAP04</v>
+      </c>
+      <c r="E15" s="5">
+        <v>6.16</v>
+      </c>
+      <c r="F15" s="5">
+        <f>E15*C15</f>
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="str">
+        <f>Sheet1!A22</f>
+        <v>118-2MS1T2B3M2QES</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16">
+        <f>Sheet1!B22</f>
+        <v>2</v>
+      </c>
+      <c r="D16" t="str">
+        <f>Sheet1!C22</f>
+        <v>Toggle Switch</v>
+      </c>
+      <c r="E16" s="5">
+        <f>Sheet1!D22</f>
+        <v>3.17</v>
+      </c>
+      <c r="F16" s="5">
+        <f>Sheet1!E22</f>
+        <v>6.34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="str">
+        <f>Sheet1!A23</f>
+        <v>538-43045-2022</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <f>Sheet1!B23</f>
+        <v>2</v>
+      </c>
+      <c r="D17" t="str">
+        <f>Sheet1!C23</f>
+        <v>Headers &amp; Wire Housings Microfit 3.0</v>
+      </c>
+      <c r="E17" s="5">
+        <f>Sheet1!D23</f>
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="F17" s="5">
+        <f>Sheet1!E23</f>
+        <v>16.420000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="str">
+        <f>Sheet1!A24</f>
+        <v>640-MEM20670218000A</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18">
+        <f>Sheet1!B24</f>
+        <v>2</v>
+      </c>
+      <c r="D18" t="str">
+        <f>Sheet1!C24</f>
+        <v>Micro SDCard Holder</v>
+      </c>
+      <c r="E18" s="5">
+        <f>Sheet1!D24</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F18" s="5">
+        <f>Sheet1!E24</f>
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19">
+        <v>4684</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="5">
+        <v>3.95</v>
+      </c>
+      <c r="F19" s="5">
+        <f>E19*C19</f>
+        <v>3.95</v>
+      </c>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1.96</v>
+      </c>
+      <c r="F20" s="5">
+        <f>E20*C20</f>
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="11">
+        <v>1.33</v>
+      </c>
+      <c r="F21" s="5">
+        <f>E21*C21</f>
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="11">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F22" s="5">
+        <f>E22*C22</f>
+        <v>8.2000000000000011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="5">
+        <f>SUM(F1:F22)</f>
+        <v>129.53200000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B27" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>